<commit_message>
Added help sheet to Excel example file
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Help" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="29">
   <si>
     <t>Cos</t>
   </si>
@@ -57,16 +58,55 @@
     <t>T20</t>
   </si>
   <si>
-    <t>Category Label 4</t>
+    <t>30-60</t>
   </si>
   <si>
-    <t>Category Label 5</t>
+    <t>DataExplorer</t>
   </si>
   <si>
-    <t>Category Label 6</t>
+    <t>A Python script for exploring your data.</t>
   </si>
   <si>
-    <t>30-60</t>
+    <t>The first row must contain the headers (names) of each column</t>
+  </si>
+  <si>
+    <t>Only the first sheet of the current workbook is read in. The contents of the other sheets (like this one) are ignored</t>
+  </si>
+  <si>
+    <t>The data must start at the second row</t>
+  </si>
+  <si>
+    <t>Columns with strings in the data are used as category columns</t>
+  </si>
+  <si>
+    <t>All other columns are used as value columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing values in value columns are allowed </t>
+  </si>
+  <si>
+    <t>Do not include any empty rows!</t>
+  </si>
+  <si>
+    <t>Missing values in category columns are not allowed</t>
+  </si>
+  <si>
+    <t>Category Label 1</t>
+  </si>
+  <si>
+    <t>Category Label 2</t>
+  </si>
+  <si>
+    <t>Category Label 3</t>
+  </si>
+  <si>
+    <t>The DataExplorer lets you filter your data by categories:</t>
+  </si>
+  <si>
+    <t>Listed here are a couple of rules you need to follow, in order to read in and view your data correctly:</t>
+  </si>
+  <si>
+    <t>Excel's time format is automatically recognized and may be used to create value columns with a time index</t>
   </si>
 </sst>
 </file>
@@ -443,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="E304" sqref="E304"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,13 +498,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -7390,7 +7430,7 @@
         <v>7</v>
       </c>
       <c r="D302" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E302">
         <v>-1</v>
@@ -7413,7 +7453,7 @@
         <v>7</v>
       </c>
       <c r="D303" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E303">
         <v>-0.98192869726270682</v>
@@ -7436,7 +7476,7 @@
         <v>7</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E304">
         <v>-0.92836793301607234</v>
@@ -7459,7 +7499,7 @@
         <v>7</v>
       </c>
       <c r="D305" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E305">
         <v>-0.84125353283118121</v>
@@ -7482,7 +7522,7 @@
         <v>7</v>
       </c>
       <c r="D306" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E306">
         <v>-0.72373403810506942</v>
@@ -7505,7 +7545,7 @@
         <v>7</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E307">
         <v>-0.58005690957119782</v>
@@ -7528,7 +7568,7 @@
         <v>7</v>
       </c>
       <c r="D308" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E308">
         <v>-0.41541501300188671</v>
@@ -7551,7 +7591,7 @@
         <v>7</v>
       </c>
       <c r="D309" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E309">
         <v>-0.2357589355094265</v>
@@ -7574,7 +7614,7 @@
         <v>7</v>
       </c>
       <c r="D310" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E310">
         <v>-4.7581915823742257E-2</v>
@@ -7597,7 +7637,7 @@
         <v>7</v>
       </c>
       <c r="D311" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E311">
         <v>0.14231483827328539</v>
@@ -7620,7 +7660,7 @@
         <v>7</v>
       </c>
       <c r="D312" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E312">
         <v>0.32706796331742199</v>
@@ -7643,7 +7683,7 @@
         <v>7</v>
       </c>
       <c r="D313" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E313">
         <v>0.49999999999999972</v>
@@ -7666,7 +7706,7 @@
         <v>7</v>
       </c>
       <c r="D314" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E314">
         <v>0.65486073394528566</v>
@@ -7689,7 +7729,7 @@
         <v>7</v>
       </c>
       <c r="D315" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E315">
         <v>0.78605309474278751</v>
@@ -7712,7 +7752,7 @@
         <v>7</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E316">
         <v>0.88883544865492359</v>
@@ -7735,7 +7775,7 @@
         <v>7</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E317">
         <v>0.95949297361449748</v>
@@ -7758,7 +7798,7 @@
         <v>7</v>
       </c>
       <c r="D318" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E318">
         <v>0.99547192257308459</v>
@@ -7781,7 +7821,7 @@
         <v>7</v>
       </c>
       <c r="D319" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E319">
         <v>0.99547192257308448</v>
@@ -7804,7 +7844,7 @@
         <v>7</v>
       </c>
       <c r="D320" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E320">
         <v>0.95949297361449737</v>
@@ -7827,7 +7867,7 @@
         <v>7</v>
       </c>
       <c r="D321" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E321">
         <v>0.88883544865492337</v>
@@ -7850,7 +7890,7 @@
         <v>7</v>
       </c>
       <c r="D322" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E322">
         <v>0.78605309474278717</v>
@@ -7873,7 +7913,7 @@
         <v>7</v>
       </c>
       <c r="D323" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E323">
         <v>0.65486073394528521</v>
@@ -7896,7 +7936,7 @@
         <v>7</v>
       </c>
       <c r="D324" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E324">
         <v>0.50000000000000011</v>
@@ -7919,7 +7959,7 @@
         <v>7</v>
       </c>
       <c r="D325" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E325">
         <v>0.32706796331742161</v>
@@ -7942,7 +7982,7 @@
         <v>7</v>
       </c>
       <c r="D326" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E326">
         <v>0.14231483827328489</v>
@@ -7965,7 +8005,7 @@
         <v>7</v>
       </c>
       <c r="D327" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E327">
         <v>-4.758191582374275E-2</v>
@@ -7988,7 +8028,7 @@
         <v>7</v>
       </c>
       <c r="D328" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E328">
         <v>-0.235758935509427</v>
@@ -8011,7 +8051,7 @@
         <v>7</v>
       </c>
       <c r="D329" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E329">
         <v>-0.41541501300188638</v>
@@ -8034,7 +8074,7 @@
         <v>7</v>
       </c>
       <c r="D330" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E330">
         <v>-0.58005690957119826</v>
@@ -8057,7 +8097,7 @@
         <v>7</v>
       </c>
       <c r="D331" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E331">
         <v>-0.72373403810507031</v>
@@ -8080,7 +8120,7 @@
         <v>7</v>
       </c>
       <c r="D332" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E332">
         <v>-0.84125353283118098</v>
@@ -8103,7 +8143,7 @@
         <v>7</v>
       </c>
       <c r="D333" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E333">
         <v>-0.92836793301607257</v>
@@ -8126,7 +8166,7 @@
         <v>7</v>
       </c>
       <c r="D334" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E334">
         <v>-0.98192869726270671</v>
@@ -8149,7 +8189,7 @@
         <v>7</v>
       </c>
       <c r="D335" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E335">
         <v>-1</v>
@@ -8172,7 +8212,7 @@
         <v>7</v>
       </c>
       <c r="D336" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E336">
         <v>-0.9819286972627066</v>
@@ -8195,7 +8235,7 @@
         <v>7</v>
       </c>
       <c r="D337" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E337">
         <v>-0.92836793301607279</v>
@@ -8218,7 +8258,7 @@
         <v>7</v>
       </c>
       <c r="D338" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E338">
         <v>-0.84125353283118132</v>
@@ -8241,7 +8281,7 @@
         <v>7</v>
       </c>
       <c r="D339" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E339">
         <v>-0.7237340381050702</v>
@@ -8264,7 +8304,7 @@
         <v>7</v>
       </c>
       <c r="D340" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E340">
         <v>-0.58005690957119804</v>
@@ -8287,7 +8327,7 @@
         <v>7</v>
       </c>
       <c r="D341" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E341">
         <v>-0.41541501300188688</v>
@@ -8310,7 +8350,7 @@
         <v>7</v>
       </c>
       <c r="D342" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E342">
         <v>-0.23575893550942759</v>
@@ -8333,7 +8373,7 @@
         <v>7</v>
       </c>
       <c r="D343" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E343">
         <v>-4.75819158237425E-2</v>
@@ -8356,7 +8396,7 @@
         <v>7</v>
       </c>
       <c r="D344" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E344">
         <v>0.14231483827328509</v>
@@ -8379,7 +8419,7 @@
         <v>7</v>
       </c>
       <c r="D345" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E345">
         <v>0.32706796331742177</v>
@@ -8402,7 +8442,7 @@
         <v>7</v>
       </c>
       <c r="D346" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E346">
         <v>0.4999999999999995</v>
@@ -8425,7 +8465,7 @@
         <v>7</v>
       </c>
       <c r="D347" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E347">
         <v>0.65486073394528543</v>
@@ -8448,7 +8488,7 @@
         <v>7</v>
       </c>
       <c r="D348" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E348">
         <v>0.78605309474278739</v>
@@ -8471,7 +8511,7 @@
         <v>7</v>
       </c>
       <c r="D349" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E349">
         <v>0.88883544865492303</v>
@@ -8494,7 +8534,7 @@
         <v>7</v>
       </c>
       <c r="D350" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E350">
         <v>0.95949297361449748</v>
@@ -8517,7 +8557,7 @@
         <v>7</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E351">
         <v>0.99547192257308459</v>
@@ -8540,7 +8580,7 @@
         <v>7</v>
       </c>
       <c r="D352" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E352">
         <v>0.99547192257308459</v>
@@ -8563,7 +8603,7 @@
         <v>7</v>
       </c>
       <c r="D353" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E353">
         <v>0.95949297361449748</v>
@@ -8586,7 +8626,7 @@
         <v>7</v>
       </c>
       <c r="D354" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E354">
         <v>0.88883544865492381</v>
@@ -8609,7 +8649,7 @@
         <v>7</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E355">
         <v>0.78605309474278739</v>
@@ -8632,7 +8672,7 @@
         <v>7</v>
       </c>
       <c r="D356" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E356">
         <v>0.65486073394528543</v>
@@ -8655,7 +8695,7 @@
         <v>7</v>
       </c>
       <c r="D357" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E357">
         <v>0.50000000000000111</v>
@@ -8678,7 +8718,7 @@
         <v>7</v>
       </c>
       <c r="D358" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E358">
         <v>0.32706796331742177</v>
@@ -8701,7 +8741,7 @@
         <v>7</v>
       </c>
       <c r="D359" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E359">
         <v>0.142314838273286</v>
@@ -8724,7 +8764,7 @@
         <v>7</v>
       </c>
       <c r="D360" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E360">
         <v>-4.75819158237425E-2</v>
@@ -8747,7 +8787,7 @@
         <v>7</v>
       </c>
       <c r="D361" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E361">
         <v>-0.23575893550942681</v>
@@ -8770,7 +8810,7 @@
         <v>7</v>
       </c>
       <c r="D362" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E362">
         <v>-0.41541501300188532</v>
@@ -8793,7 +8833,7 @@
         <v>7</v>
       </c>
       <c r="D363" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E363">
         <v>-0.58005690957119804</v>
@@ -8816,7 +8856,7 @@
         <v>7</v>
       </c>
       <c r="D364" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E364">
         <v>-0.72373403810506953</v>
@@ -8839,7 +8879,7 @@
         <v>7</v>
       </c>
       <c r="D365" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E365">
         <v>-0.84125353283118132</v>
@@ -8862,7 +8902,7 @@
         <v>7</v>
       </c>
       <c r="D366" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E366">
         <v>-0.92836793301607246</v>
@@ -8885,7 +8925,7 @@
         <v>7</v>
       </c>
       <c r="D367" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E367">
         <v>-0.98192869726270648</v>
@@ -8908,7 +8948,7 @@
         <v>7</v>
       </c>
       <c r="D368" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E368">
         <v>-1</v>
@@ -8931,7 +8971,7 @@
         <v>7</v>
       </c>
       <c r="D369" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E369">
         <v>-0.98192869726270682</v>
@@ -8954,7 +8994,7 @@
         <v>7</v>
       </c>
       <c r="D370" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E370">
         <v>-0.92836793301607257</v>
@@ -8977,7 +9017,7 @@
         <v>7</v>
       </c>
       <c r="D371" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E371">
         <v>-0.84125353283118143</v>
@@ -9000,7 +9040,7 @@
         <v>7</v>
       </c>
       <c r="D372" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E372">
         <v>-0.72373403810507098</v>
@@ -9023,7 +9063,7 @@
         <v>7</v>
       </c>
       <c r="D373" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E373">
         <v>-0.58005690957119826</v>
@@ -9046,7 +9086,7 @@
         <v>7</v>
       </c>
       <c r="D374" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E374">
         <v>-0.41541501300188721</v>
@@ -9069,7 +9109,7 @@
         <v>7</v>
       </c>
       <c r="D375" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E375">
         <v>-0.235758935509427</v>
@@ -9092,7 +9132,7 @@
         <v>7</v>
       </c>
       <c r="D376" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E376">
         <v>-4.758191582374275E-2</v>
@@ -9115,7 +9155,7 @@
         <v>7</v>
       </c>
       <c r="D377" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E377">
         <v>0.14231483827328401</v>
@@ -9138,7 +9178,7 @@
         <v>7</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E378">
         <v>0.32706796331742161</v>
@@ -9161,7 +9201,7 @@
         <v>7</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E379">
         <v>0.49999999999999928</v>
@@ -9184,7 +9224,7 @@
         <v>7</v>
       </c>
       <c r="D380" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E380">
         <v>0.65486073394528388</v>
@@ -9207,7 +9247,7 @@
         <v>7</v>
       </c>
       <c r="D381" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E381">
         <v>0.78605309474278717</v>
@@ -9230,7 +9270,7 @@
         <v>7</v>
       </c>
       <c r="D382" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E382">
         <v>0.88883544865492292</v>
@@ -9253,7 +9293,7 @@
         <v>7</v>
       </c>
       <c r="D383" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E383">
         <v>0.95949297361449737</v>
@@ -9276,7 +9316,7 @@
         <v>7</v>
       </c>
       <c r="D384" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E384">
         <v>0.99547192257308448</v>
@@ -9299,7 +9339,7 @@
         <v>7</v>
       </c>
       <c r="D385" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E385">
         <v>0.9954719225730847</v>
@@ -9322,7 +9362,7 @@
         <v>7</v>
       </c>
       <c r="D386" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E386">
         <v>0.95949297361449748</v>
@@ -9345,7 +9385,7 @@
         <v>7</v>
       </c>
       <c r="D387" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E387">
         <v>0.88883544865492403</v>
@@ -9368,7 +9408,7 @@
         <v>7</v>
       </c>
       <c r="D388" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E388">
         <v>0.78605309474278751</v>
@@ -9391,7 +9431,7 @@
         <v>7</v>
       </c>
       <c r="D389" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E389">
         <v>0.65486073394528699</v>
@@ -9414,7 +9454,7 @@
         <v>7</v>
       </c>
       <c r="D390" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E390">
         <v>0.50000000000000122</v>
@@ -9437,7 +9477,7 @@
         <v>7</v>
       </c>
       <c r="D391" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E391">
         <v>0.32706796331742199</v>
@@ -9460,7 +9500,7 @@
         <v>7</v>
       </c>
       <c r="D392" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E392">
         <v>0.14231483827328451</v>
@@ -9483,7 +9523,7 @@
         <v>7</v>
       </c>
       <c r="D393" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E393">
         <v>-4.7581915823740481E-2</v>
@@ -9506,7 +9546,7 @@
         <v>7</v>
       </c>
       <c r="D394" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E394">
         <v>-0.2357589355094265</v>
@@ -9529,7 +9569,7 @@
         <v>7</v>
       </c>
       <c r="D395" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E395">
         <v>-0.41541501300188671</v>
@@ -9552,7 +9592,7 @@
         <v>7</v>
       </c>
       <c r="D396" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E396">
         <v>-0.58005690957119638</v>
@@ -9575,7 +9615,7 @@
         <v>7</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E397">
         <v>-0.72373403810506942</v>
@@ -9598,7 +9638,7 @@
         <v>7</v>
       </c>
       <c r="D398" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E398">
         <v>-0.84125353283118121</v>
@@ -9621,7 +9661,7 @@
         <v>7</v>
       </c>
       <c r="D399" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E399">
         <v>-0.92836793301607168</v>
@@ -9644,7 +9684,7 @@
         <v>7</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E400">
         <v>-0.98192869726270637</v>
@@ -9667,7 +9707,7 @@
         <v>7</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E401">
         <v>-1</v>
@@ -9690,7 +9730,7 @@
         <v>6</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F402">
         <v>1</v>
@@ -9713,7 +9753,7 @@
         <v>6</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F403">
         <v>0.99547192257308459</v>
@@ -9736,7 +9776,7 @@
         <v>6</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F404">
         <v>0.9819286972627066</v>
@@ -9759,7 +9799,7 @@
         <v>6</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F405">
         <v>0.95949297361449737</v>
@@ -9782,7 +9822,7 @@
         <v>6</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F406">
         <v>0.92836793301607246</v>
@@ -9805,7 +9845,7 @@
         <v>6</v>
       </c>
       <c r="D407" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F407">
         <v>0.88883544865492337</v>
@@ -9828,7 +9868,7 @@
         <v>6</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F408">
         <v>0.84125353283118132</v>
@@ -9851,7 +9891,7 @@
         <v>6</v>
       </c>
       <c r="D409" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F409">
         <v>0.78605309474278728</v>
@@ -9874,7 +9914,7 @@
         <v>6</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F410">
         <v>0.7237340381050702</v>
@@ -9897,7 +9937,7 @@
         <v>6</v>
       </c>
       <c r="D411" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F411">
         <v>0.65486073394528499</v>
@@ -9920,7 +9960,7 @@
         <v>6</v>
       </c>
       <c r="D412" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F412">
         <v>0.58005690957119804</v>
@@ -9943,7 +9983,7 @@
         <v>6</v>
       </c>
       <c r="D413" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F413">
         <v>0.50000000000000011</v>
@@ -9966,7 +10006,7 @@
         <v>6</v>
       </c>
       <c r="D414" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F414">
         <v>0.4154150130018861</v>
@@ -9989,7 +10029,7 @@
         <v>6</v>
       </c>
       <c r="D415" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F415">
         <v>0.32706796331742161</v>
@@ -10012,7 +10052,7 @@
         <v>6</v>
       </c>
       <c r="D416" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F416">
         <v>0.23575893550942709</v>
@@ -10035,7 +10075,7 @@
         <v>6</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F417">
         <v>0.14231483827328489</v>
@@ -10058,7 +10098,7 @@
         <v>6</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F418">
         <v>4.7581915823742438E-2</v>
@@ -10081,7 +10121,7 @@
         <v>6</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F419">
         <v>-4.7581915823742688E-2</v>
@@ -10104,7 +10144,7 @@
         <v>6</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F420">
         <v>-0.1423148382732852</v>
@@ -10127,7 +10167,7 @@
         <v>6</v>
       </c>
       <c r="D421" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F421">
         <v>-0.23575893550942739</v>
@@ -10150,7 +10190,7 @@
         <v>6</v>
       </c>
       <c r="D422" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F422">
         <v>-0.32706796331742177</v>
@@ -10173,7 +10213,7 @@
         <v>6</v>
       </c>
       <c r="D423" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F423">
         <v>-0.41541501300188632</v>
@@ -10196,7 +10236,7 @@
         <v>6</v>
       </c>
       <c r="D424" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F424">
         <v>-0.49999999999999989</v>
@@ -10219,7 +10259,7 @@
         <v>6</v>
       </c>
       <c r="D425" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F425">
         <v>-0.58005690957119826</v>
@@ -10242,7 +10282,7 @@
         <v>6</v>
       </c>
       <c r="D426" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F426">
         <v>-0.65486073394528521</v>
@@ -10265,7 +10305,7 @@
         <v>6</v>
       </c>
       <c r="D427" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F427">
         <v>-0.72373403810507031</v>
@@ -10288,7 +10328,7 @@
         <v>6</v>
       </c>
       <c r="D428" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F428">
         <v>-0.78605309474278739</v>
@@ -10311,7 +10351,7 @@
         <v>6</v>
       </c>
       <c r="D429" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F429">
         <v>-0.84125353283118109</v>
@@ -10334,7 +10374,7 @@
         <v>6</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F430">
         <v>-0.88883544865492348</v>
@@ -10357,7 +10397,7 @@
         <v>6</v>
       </c>
       <c r="D431" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F431">
         <v>-0.92836793301607268</v>
@@ -10380,7 +10420,7 @@
         <v>6</v>
       </c>
       <c r="D432" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F432">
         <v>-0.95949297361449737</v>
@@ -10403,7 +10443,7 @@
         <v>6</v>
       </c>
       <c r="D433" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F433">
         <v>-0.98192869726270671</v>
@@ -10426,7 +10466,7 @@
         <v>6</v>
       </c>
       <c r="D434" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F434">
         <v>-0.99547192257308459</v>
@@ -10449,7 +10489,7 @@
         <v>6</v>
       </c>
       <c r="D435" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F435">
         <v>-1</v>
@@ -10472,7 +10512,7 @@
         <v>6</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F436">
         <v>-0.99547192257308459</v>
@@ -10495,7 +10535,7 @@
         <v>6</v>
       </c>
       <c r="D437" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F437">
         <v>-0.98192869726270671</v>
@@ -10518,7 +10558,7 @@
         <v>6</v>
       </c>
       <c r="D438" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F438">
         <v>-0.95949297361449737</v>
@@ -10541,7 +10581,7 @@
         <v>6</v>
       </c>
       <c r="D439" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F439">
         <v>-0.92836793301607257</v>
@@ -10564,7 +10604,7 @@
         <v>6</v>
       </c>
       <c r="D440" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F440">
         <v>-0.88883544865492348</v>
@@ -10587,7 +10627,7 @@
         <v>6</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F441">
         <v>-0.84125353283118132</v>
@@ -10610,7 +10650,7 @@
         <v>6</v>
       </c>
       <c r="D442" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F442">
         <v>-0.78605309474278762</v>
@@ -10633,7 +10673,7 @@
         <v>6</v>
       </c>
       <c r="D443" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F443">
         <v>-0.7237340381050702</v>
@@ -10656,7 +10696,7 @@
         <v>6</v>
       </c>
       <c r="D444" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F444">
         <v>-0.6548607339452851</v>
@@ -10679,7 +10719,7 @@
         <v>6</v>
       </c>
       <c r="D445" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F445">
         <v>-0.58005690957119815</v>
@@ -10702,7 +10742,7 @@
         <v>6</v>
       </c>
       <c r="D446" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F446">
         <v>-0.50000000000000022</v>
@@ -10725,7 +10765,7 @@
         <v>6</v>
       </c>
       <c r="D447" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F447">
         <v>-0.41541501300188621</v>
@@ -10748,7 +10788,7 @@
         <v>6</v>
       </c>
       <c r="D448" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F448">
         <v>-0.32706796331742172</v>
@@ -10771,7 +10811,7 @@
         <v>6</v>
       </c>
       <c r="D449" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F449">
         <v>-0.2357589355094277</v>
@@ -10794,7 +10834,7 @@
         <v>6</v>
       </c>
       <c r="D450" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F450">
         <v>-0.14231483827328509</v>
@@ -10817,7 +10857,7 @@
         <v>6</v>
       </c>
       <c r="D451" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F451">
         <v>-4.7581915823742563E-2</v>
@@ -10840,7 +10880,7 @@
         <v>6</v>
       </c>
       <c r="D452" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F452">
         <v>4.7581915823742563E-2</v>
@@ -10863,7 +10903,7 @@
         <v>6</v>
       </c>
       <c r="D453" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F453">
         <v>0.14231483827328509</v>
@@ -10886,7 +10926,7 @@
         <v>6</v>
       </c>
       <c r="D454" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F454">
         <v>0.23575893550942681</v>
@@ -10909,7 +10949,7 @@
         <v>6</v>
       </c>
       <c r="D455" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F455">
         <v>0.32706796331742172</v>
@@ -10932,7 +10972,7 @@
         <v>6</v>
       </c>
       <c r="D456" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F456">
         <v>0.41541501300188621</v>
@@ -10955,7 +10995,7 @@
         <v>6</v>
       </c>
       <c r="D457" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F457">
         <v>0.49999999999999939</v>
@@ -10978,7 +11018,7 @@
         <v>6</v>
       </c>
       <c r="D458" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F458">
         <v>0.58005690957119815</v>
@@ -11001,7 +11041,7 @@
         <v>6</v>
       </c>
       <c r="D459" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F459">
         <v>0.65486073394528477</v>
@@ -11024,7 +11064,7 @@
         <v>6</v>
       </c>
       <c r="D460" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F460">
         <v>0.7237340381050702</v>
@@ -11047,7 +11087,7 @@
         <v>6</v>
       </c>
       <c r="D461" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F461">
         <v>0.78605309474278728</v>
@@ -11070,7 +11110,7 @@
         <v>6</v>
       </c>
       <c r="D462" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F462">
         <v>0.84125353283118087</v>
@@ -11093,7 +11133,7 @@
         <v>6</v>
       </c>
       <c r="D463" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F463">
         <v>0.88883544865492348</v>
@@ -11116,7 +11156,7 @@
         <v>6</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F464">
         <v>0.92836793301607246</v>
@@ -11139,7 +11179,7 @@
         <v>6</v>
       </c>
       <c r="D465" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F465">
         <v>0.95949297361449737</v>
@@ -11162,7 +11202,7 @@
         <v>6</v>
       </c>
       <c r="D466" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F466">
         <v>0.98192869726270671</v>
@@ -11185,7 +11225,7 @@
         <v>6</v>
       </c>
       <c r="D467" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F467">
         <v>0.99547192257308459</v>
@@ -11208,7 +11248,7 @@
         <v>6</v>
       </c>
       <c r="D468" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F468">
         <v>1</v>
@@ -11231,7 +11271,7 @@
         <v>6</v>
       </c>
       <c r="D469" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F469">
         <v>0.99547192257308459</v>
@@ -11254,7 +11294,7 @@
         <v>6</v>
       </c>
       <c r="D470" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F470">
         <v>0.98192869726270671</v>
@@ -11277,7 +11317,7 @@
         <v>6</v>
       </c>
       <c r="D471" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F471">
         <v>0.95949297361449748</v>
@@ -11300,7 +11340,7 @@
         <v>6</v>
       </c>
       <c r="D472" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F472">
         <v>0.92836793301607279</v>
@@ -11323,7 +11363,7 @@
         <v>6</v>
       </c>
       <c r="D473" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F473">
         <v>0.88883544865492348</v>
@@ -11346,7 +11386,7 @@
         <v>6</v>
       </c>
       <c r="D474" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F474">
         <v>0.84125353283118143</v>
@@ -11369,7 +11409,7 @@
         <v>6</v>
       </c>
       <c r="D475" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F475">
         <v>0.78605309474278739</v>
@@ -11392,7 +11432,7 @@
         <v>6</v>
       </c>
       <c r="D476" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F476">
         <v>0.72373403810507031</v>
@@ -11415,7 +11455,7 @@
         <v>6</v>
       </c>
       <c r="D477" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F477">
         <v>0.65486073394528554</v>
@@ -11438,7 +11478,7 @@
         <v>6</v>
       </c>
       <c r="D478" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F478">
         <v>0.58005690957119826</v>
@@ -11461,7 +11501,7 @@
         <v>6</v>
       </c>
       <c r="D479" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F479">
         <v>0.50000000000000033</v>
@@ -11484,7 +11524,7 @@
         <v>6</v>
       </c>
       <c r="D480" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F480">
         <v>0.4154150130018871</v>
@@ -11507,7 +11547,7 @@
         <v>6</v>
       </c>
       <c r="D481" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F481">
         <v>0.32706796331742177</v>
@@ -11530,7 +11570,7 @@
         <v>6</v>
       </c>
       <c r="D482" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F482">
         <v>0.23575893550942781</v>
@@ -11553,7 +11593,7 @@
         <v>6</v>
       </c>
       <c r="D483" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F483">
         <v>0.1423148382732852</v>
@@ -11576,7 +11616,7 @@
         <v>6</v>
       </c>
       <c r="D484" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F484">
         <v>4.7581915823742688E-2</v>
@@ -11599,7 +11639,7 @@
         <v>6</v>
       </c>
       <c r="D485" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F485">
         <v>-4.7581915823741557E-2</v>
@@ -11622,7 +11662,7 @@
         <v>6</v>
       </c>
       <c r="D486" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F486">
         <v>-0.14231483827328489</v>
@@ -11645,7 +11685,7 @@
         <v>6</v>
       </c>
       <c r="D487" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F487">
         <v>-0.2357589355094267</v>
@@ -11668,7 +11708,7 @@
         <v>6</v>
       </c>
       <c r="D488" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F488">
         <v>-0.32706796331742161</v>
@@ -11691,7 +11731,7 @@
         <v>6</v>
       </c>
       <c r="D489" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F489">
         <v>-0.41541501300188532</v>
@@ -11714,7 +11754,7 @@
         <v>6</v>
       </c>
       <c r="D490" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F490">
         <v>-0.49999999999999928</v>
@@ -11737,7 +11777,7 @@
         <v>6</v>
       </c>
       <c r="D491" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F491">
         <v>-0.58005690957119804</v>
@@ -11760,7 +11800,7 @@
         <v>6</v>
       </c>
       <c r="D492" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F492">
         <v>-0.65486073394528532</v>
@@ -11783,7 +11823,7 @@
         <v>6</v>
       </c>
       <c r="D493" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F493">
         <v>-0.72373403810506953</v>
@@ -11806,7 +11846,7 @@
         <v>6</v>
       </c>
       <c r="D494" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F494">
         <v>-0.78605309474278728</v>
@@ -11829,7 +11869,7 @@
         <v>6</v>
       </c>
       <c r="D495" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F495">
         <v>-0.84125353283118132</v>
@@ -11852,7 +11892,7 @@
         <v>6</v>
       </c>
       <c r="D496" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F496">
         <v>-0.88883544865492292</v>
@@ -11875,7 +11915,7 @@
         <v>6</v>
       </c>
       <c r="D497" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F497">
         <v>-0.92836793301607246</v>
@@ -11898,7 +11938,7 @@
         <v>6</v>
       </c>
       <c r="D498" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F498">
         <v>-0.95949297361449737</v>
@@ -11921,7 +11961,7 @@
         <v>6</v>
       </c>
       <c r="D499" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F499">
         <v>-0.98192869726270648</v>
@@ -11944,7 +11984,7 @@
         <v>6</v>
       </c>
       <c r="D500" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F500">
         <v>-0.99547192257308459</v>
@@ -11967,7 +12007,7 @@
         <v>6</v>
       </c>
       <c r="D501" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F501">
         <v>-1</v>
@@ -11990,7 +12030,7 @@
         <v>7</v>
       </c>
       <c r="D502" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E502">
         <v>-1.8369701987210299E-16</v>
@@ -12013,7 +12053,7 @@
         <v>7</v>
       </c>
       <c r="D503" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E503">
         <v>-9.5056043304182491E-2</v>
@@ -12036,7 +12076,7 @@
         <v>7</v>
       </c>
       <c r="D504" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E504">
         <v>-0.1892512443604106</v>
@@ -12059,7 +12099,7 @@
         <v>7</v>
       </c>
       <c r="D505" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E505">
         <v>-0.28173255684142973</v>
@@ -12082,7 +12122,7 @@
         <v>7</v>
       </c>
       <c r="D506" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E506">
         <v>-0.37166245566032802</v>
@@ -12105,7 +12145,7 @@
         <v>7</v>
       </c>
       <c r="D507" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E507">
         <v>-0.45822652172741057</v>
@@ -12128,7 +12168,7 @@
         <v>7</v>
       </c>
       <c r="D508" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E508">
         <v>-0.54064081745559744</v>
@@ -12151,7 +12191,7 @@
         <v>7</v>
       </c>
       <c r="D509" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E509">
         <v>-0.6181589862206055</v>
@@ -12174,7 +12214,7 @@
         <v>7</v>
       </c>
       <c r="D510" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E510">
         <v>-0.69007901148211204</v>
@@ -12197,7 +12237,7 @@
         <v>7</v>
       </c>
       <c r="D511" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E511">
         <v>-0.75574957435425838</v>
@@ -12220,7 +12260,7 @@
         <v>7</v>
       </c>
       <c r="D512" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E512">
         <v>-0.81457595205033584</v>
@@ -12243,7 +12283,7 @@
         <v>7</v>
       </c>
       <c r="D513" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E513">
         <v>-0.8660254037844386</v>
@@ -12266,7 +12306,7 @@
         <v>7</v>
       </c>
       <c r="D514" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E514">
         <v>-0.90963199535451855</v>
@@ -12289,7 +12329,7 @@
         <v>7</v>
       </c>
       <c r="D515" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E515">
         <v>-0.94500081871466846</v>
@@ -12312,7 +12352,7 @@
         <v>7</v>
       </c>
       <c r="D516" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E516">
         <v>-0.97181156832354176</v>
@@ -12335,7 +12375,7 @@
         <v>7</v>
       </c>
       <c r="D517" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E517">
         <v>-0.9898214418809328</v>
@@ -12358,7 +12398,7 @@
         <v>7</v>
       </c>
       <c r="D518" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E518">
         <v>-0.99886733918300796</v>
@@ -12381,7 +12421,7 @@
         <v>7</v>
       </c>
       <c r="D519" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E519">
         <v>-0.99886733918300796</v>
@@ -12404,7 +12444,7 @@
         <v>7</v>
       </c>
       <c r="D520" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E520">
         <v>-0.98982144188093268</v>
@@ -12427,7 +12467,7 @@
         <v>7</v>
       </c>
       <c r="D521" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E521">
         <v>-0.97181156832354165</v>
@@ -12450,7 +12490,7 @@
         <v>7</v>
       </c>
       <c r="D522" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E522">
         <v>-0.94500081871466846</v>
@@ -12473,7 +12513,7 @@
         <v>7</v>
       </c>
       <c r="D523" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E523">
         <v>-0.90963199535451844</v>
@@ -12496,7 +12536,7 @@
         <v>7</v>
       </c>
       <c r="D524" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E524">
         <v>-0.86602540378443871</v>
@@ -12519,7 +12559,7 @@
         <v>7</v>
       </c>
       <c r="D525" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E525">
         <v>-0.81457595205033573</v>
@@ -12542,7 +12582,7 @@
         <v>7</v>
       </c>
       <c r="D526" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E526">
         <v>-0.75574957435425816</v>
@@ -12565,7 +12605,7 @@
         <v>7</v>
       </c>
       <c r="D527" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E527">
         <v>-0.69007901148211181</v>
@@ -12588,7 +12628,7 @@
         <v>7</v>
       </c>
       <c r="D528" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E528">
         <v>-0.61815898622060528</v>
@@ -12611,7 +12651,7 @@
         <v>7</v>
       </c>
       <c r="D529" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E529">
         <v>-0.54064081745559756</v>
@@ -12634,7 +12674,7 @@
         <v>7</v>
       </c>
       <c r="D530" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E530">
         <v>-0.45822652172741041</v>
@@ -12657,7 +12697,7 @@
         <v>7</v>
       </c>
       <c r="D531" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E531">
         <v>-0.37166245566032741</v>
@@ -12680,7 +12720,7 @@
         <v>7</v>
       </c>
       <c r="D532" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E532">
         <v>-0.28173255684142989</v>
@@ -12703,7 +12743,7 @@
         <v>7</v>
       </c>
       <c r="D533" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E533">
         <v>-0.1892512443604103</v>
@@ -12726,7 +12766,7 @@
         <v>7</v>
       </c>
       <c r="D534" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E534">
         <v>-9.50560433041827E-2</v>
@@ -12749,7 +12789,7 @@
         <v>7</v>
       </c>
       <c r="D535" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E535">
         <v>6.123233995736766E-17</v>
@@ -12772,7 +12812,7 @@
         <v>7</v>
       </c>
       <c r="D536" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E536">
         <v>9.5056043304182811E-2</v>
@@ -12795,7 +12835,7 @@
         <v>7</v>
       </c>
       <c r="D537" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E537">
         <v>0.18925124436040999</v>
@@ -12818,7 +12858,7 @@
         <v>7</v>
       </c>
       <c r="D538" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E538">
         <v>0.28173255684142962</v>
@@ -12841,7 +12881,7 @@
         <v>7</v>
       </c>
       <c r="D539" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E539">
         <v>0.37166245566032752</v>
@@ -12864,7 +12904,7 @@
         <v>7</v>
       </c>
       <c r="D540" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E540">
         <v>0.45822652172741052</v>
@@ -12887,7 +12927,7 @@
         <v>7</v>
       </c>
       <c r="D541" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E541">
         <v>0.54064081745559733</v>
@@ -12910,7 +12950,7 @@
         <v>7</v>
       </c>
       <c r="D542" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E542">
         <v>0.61815898622060506</v>
@@ -12933,7 +12973,7 @@
         <v>7</v>
       </c>
       <c r="D543" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E543">
         <v>0.69007901148211193</v>
@@ -12956,7 +12996,7 @@
         <v>7</v>
       </c>
       <c r="D544" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E544">
         <v>0.75574957435425827</v>
@@ -12979,7 +13019,7 @@
         <v>7</v>
       </c>
       <c r="D545" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E545">
         <v>0.81457595205033573</v>
@@ -13002,7 +13042,7 @@
         <v>7</v>
       </c>
       <c r="D546" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E546">
         <v>0.86602540378443849</v>
@@ -13025,7 +13065,7 @@
         <v>7</v>
       </c>
       <c r="D547" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E547">
         <v>0.90963199535451844</v>
@@ -13048,7 +13088,7 @@
         <v>7</v>
       </c>
       <c r="D548" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E548">
         <v>0.94500081871466846</v>
@@ -13071,7 +13111,7 @@
         <v>7</v>
       </c>
       <c r="D549" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E549">
         <v>0.97181156832354154</v>
@@ -13094,7 +13134,7 @@
         <v>7</v>
       </c>
       <c r="D550" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E550">
         <v>0.9898214418809328</v>
@@ -13117,7 +13157,7 @@
         <v>7</v>
       </c>
       <c r="D551" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E551">
         <v>0.99886733918300796</v>
@@ -13140,7 +13180,7 @@
         <v>7</v>
       </c>
       <c r="D552" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E552">
         <v>0.99886733918300796</v>
@@ -13163,7 +13203,7 @@
         <v>7</v>
       </c>
       <c r="D553" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E553">
         <v>0.9898214418809328</v>
@@ -13186,7 +13226,7 @@
         <v>7</v>
       </c>
       <c r="D554" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E554">
         <v>0.97181156832354176</v>
@@ -13209,7 +13249,7 @@
         <v>7</v>
       </c>
       <c r="D555" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E555">
         <v>0.94500081871466846</v>
@@ -13232,7 +13272,7 @@
         <v>7</v>
       </c>
       <c r="D556" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E556">
         <v>0.90963199535451844</v>
@@ -13255,7 +13295,7 @@
         <v>7</v>
       </c>
       <c r="D557" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E557">
         <v>0.86602540378443893</v>
@@ -13278,7 +13318,7 @@
         <v>7</v>
       </c>
       <c r="D558" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E558">
         <v>0.81457595205033573</v>
@@ -13301,7 +13341,7 @@
         <v>7</v>
       </c>
       <c r="D559" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E559">
         <v>0.7557495743542586</v>
@@ -13324,7 +13364,7 @@
         <v>7</v>
       </c>
       <c r="D560" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E560">
         <v>0.69007901148211193</v>
@@ -13347,7 +13387,7 @@
         <v>7</v>
       </c>
       <c r="D561" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E561">
         <v>0.61815898622060539</v>
@@ -13370,7 +13410,7 @@
         <v>7</v>
       </c>
       <c r="D562" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E562">
         <v>0.54064081745559811</v>
@@ -13393,7 +13433,7 @@
         <v>7</v>
       </c>
       <c r="D563" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E563">
         <v>0.45822652172741052</v>
@@ -13416,7 +13456,7 @@
         <v>7</v>
       </c>
       <c r="D564" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E564">
         <v>0.37166245566032791</v>
@@ -13439,7 +13479,7 @@
         <v>7</v>
       </c>
       <c r="D565" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E565">
         <v>0.28173255684142962</v>
@@ -13462,7 +13502,7 @@
         <v>7</v>
       </c>
       <c r="D566" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E566">
         <v>0.18925124436041041</v>
@@ -13485,7 +13525,7 @@
         <v>7</v>
       </c>
       <c r="D567" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E567">
         <v>9.5056043304183255E-2</v>
@@ -13508,7 +13548,7 @@
         <v>7</v>
       </c>
       <c r="D568" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E568">
         <v>6.123233995736766E-17</v>
@@ -13531,7 +13571,7 @@
         <v>7</v>
       </c>
       <c r="D569" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E569">
         <v>-9.5056043304182256E-2</v>
@@ -13554,7 +13594,7 @@
         <v>7</v>
       </c>
       <c r="D570" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E570">
         <v>-0.1892512443604103</v>
@@ -13577,7 +13617,7 @@
         <v>7</v>
       </c>
       <c r="D571" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E571">
         <v>-0.28173255684142939</v>
@@ -13600,7 +13640,7 @@
         <v>7</v>
       </c>
       <c r="D572" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E572">
         <v>-0.37166245566032702</v>
@@ -13623,7 +13663,7 @@
         <v>7</v>
       </c>
       <c r="D573" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E573">
         <v>-0.45822652172741041</v>
@@ -13646,7 +13686,7 @@
         <v>7</v>
       </c>
       <c r="D574" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E574">
         <v>-0.54064081745559722</v>
@@ -13669,7 +13709,7 @@
         <v>7</v>
       </c>
       <c r="D575" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E575">
         <v>-0.61815898622060528</v>
@@ -13692,7 +13732,7 @@
         <v>7</v>
       </c>
       <c r="D576" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E576">
         <v>-0.69007901148211181</v>
@@ -13715,7 +13755,7 @@
         <v>7</v>
       </c>
       <c r="D577" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E577">
         <v>-0.75574957435425794</v>
@@ -13738,7 +13778,7 @@
         <v>7</v>
       </c>
       <c r="D578" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E578">
         <v>-0.81457595205033573</v>
@@ -13761,7 +13801,7 @@
         <v>7</v>
       </c>
       <c r="D579" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E579">
         <v>-0.86602540378443849</v>
@@ -13784,7 +13824,7 @@
         <v>7</v>
       </c>
       <c r="D580" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E580">
         <v>-0.90963199535451811</v>
@@ -13807,7 +13847,7 @@
         <v>7</v>
       </c>
       <c r="D581" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E581">
         <v>-0.94500081871466846</v>
@@ -13830,7 +13870,7 @@
         <v>7</v>
       </c>
       <c r="D582" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E582">
         <v>-0.97181156832354154</v>
@@ -13853,7 +13893,7 @@
         <v>7</v>
       </c>
       <c r="D583" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E583">
         <v>-0.98982144188093268</v>
@@ -13876,7 +13916,7 @@
         <v>7</v>
       </c>
       <c r="D584" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E584">
         <v>-0.99886733918300796</v>
@@ -13899,7 +13939,7 @@
         <v>7</v>
       </c>
       <c r="D585" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E585">
         <v>-0.99886733918300796</v>
@@ -13922,7 +13962,7 @@
         <v>7</v>
       </c>
       <c r="D586" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E586">
         <v>-0.9898214418809328</v>
@@ -13945,7 +13985,7 @@
         <v>7</v>
       </c>
       <c r="D587" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E587">
         <v>-0.97181156832354187</v>
@@ -13968,7 +14008,7 @@
         <v>7</v>
       </c>
       <c r="D588" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E588">
         <v>-0.94500081871466846</v>
@@ -13991,7 +14031,7 @@
         <v>7</v>
       </c>
       <c r="D589" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E589">
         <v>-0.90963199535451889</v>
@@ -14014,7 +14054,7 @@
         <v>7</v>
       </c>
       <c r="D590" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E590">
         <v>-0.86602540378443904</v>
@@ -14037,7 +14077,7 @@
         <v>7</v>
       </c>
       <c r="D591" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E591">
         <v>-0.81457595205033584</v>
@@ -14060,7 +14100,7 @@
         <v>7</v>
       </c>
       <c r="D592" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E592">
         <v>-0.75574957435425805</v>
@@ -14083,7 +14123,7 @@
         <v>7</v>
       </c>
       <c r="D593" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E593">
         <v>-0.69007901148211259</v>
@@ -14106,7 +14146,7 @@
         <v>7</v>
       </c>
       <c r="D594" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E594">
         <v>-0.6181589862206055</v>
@@ -14129,7 +14169,7 @@
         <v>7</v>
       </c>
       <c r="D595" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E595">
         <v>-0.54064081745559744</v>
@@ -14152,7 +14192,7 @@
         <v>7</v>
       </c>
       <c r="D596" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E596">
         <v>-0.45822652172741141</v>
@@ -14175,7 +14215,7 @@
         <v>7</v>
       </c>
       <c r="D597" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E597">
         <v>-0.37166245566032802</v>
@@ -14198,7 +14238,7 @@
         <v>7</v>
       </c>
       <c r="D598" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E598">
         <v>-0.28173255684142973</v>
@@ -14221,7 +14261,7 @@
         <v>7</v>
       </c>
       <c r="D599" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E599">
         <v>-0.18925124436041141</v>
@@ -14244,7 +14284,7 @@
         <v>7</v>
       </c>
       <c r="D600" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E600">
         <v>-9.505604330418338E-2</v>
@@ -14267,7 +14307,7 @@
         <v>7</v>
       </c>
       <c r="D601" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E601">
         <v>-1.8369701987210299E-16</v>
@@ -14282,4 +14322,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>